<commit_message>
modifs - 5 done
</commit_message>
<xml_diff>
--- a/Volume_and_morphosource_ID.xlsx
+++ b/Volume_and_morphosource_ID.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document_UQAR\These\chapitre_1\Article\Soumission\raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document_UQAR\These\chapitre_1\Article\projet_git_hub\Raw_data_Axolotl_Brains\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF9F3424-500A-4656-AC8A-37D8DE134520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3594A55D-600D-4C0E-AED4-04C44D0165DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="188">
   <si>
     <t>ID</t>
   </si>
@@ -583,6 +583,12 @@
   </si>
   <si>
     <t>https://www.morphosource.org/concern/media/000780068?locale=en</t>
+  </si>
+  <si>
+    <t>000780098</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780098?locale=en</t>
   </si>
 </sst>
 </file>
@@ -922,7 +928,7 @@
   <dimension ref="A1:N999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1154,6 +1160,12 @@
       </c>
       <c r="L5" s="4">
         <v>0.33668427550000002</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>186</v>
+      </c>
+      <c r="N5" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
morphosource D10 - 10 done
</commit_message>
<xml_diff>
--- a/Volume_and_morphosource_ID.xlsx
+++ b/Volume_and_morphosource_ID.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Document_UQAR\These\chapitre_1\Article\projet_git_hub\Raw_data_Axolotl_Brains\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3594A55D-600D-4C0E-AED4-04C44D0165DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D13DD12-709D-475D-B143-2CA1FF7F4CFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="200">
   <si>
     <t>ID</t>
   </si>
@@ -589,6 +589,42 @@
   </si>
   <si>
     <t>https://www.morphosource.org/concern/media/000780098?locale=en</t>
+  </si>
+  <si>
+    <t>000780107</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780107?locale=en</t>
+  </si>
+  <si>
+    <t>000780112</t>
+  </si>
+  <si>
+    <t>000780332</t>
+  </si>
+  <si>
+    <t>000780389</t>
+  </si>
+  <si>
+    <t>000780394</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780112?locale=en</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780332?locale=en</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780389?locale=en</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780394?locale=en</t>
+  </si>
+  <si>
+    <t>000780399</t>
+  </si>
+  <si>
+    <t>https://www.morphosource.org/concern/media/000780399?locale=en</t>
   </si>
 </sst>
 </file>
@@ -674,7 +710,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -707,6 +743,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,8 +964,8 @@
   </sheetPr>
   <dimension ref="A1:N999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1205,6 +1242,12 @@
       <c r="L6" s="4">
         <v>0.33261599149999999</v>
       </c>
+      <c r="M6" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="N6" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -1243,6 +1286,12 @@
       <c r="L7" s="4">
         <v>0.35054236370000003</v>
       </c>
+      <c r="M7" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="N7" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1281,6 +1330,12 @@
       <c r="L8" s="4">
         <v>0.35753703409999998</v>
       </c>
+      <c r="M8" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="N8" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1319,6 +1374,12 @@
       <c r="L9" s="4">
         <v>0.29190033780000002</v>
       </c>
+      <c r="M9" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="N9" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1357,6 +1418,12 @@
       <c r="L10" s="4">
         <v>0.30504747430000001</v>
       </c>
+      <c r="M10" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="N10" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1394,6 +1461,12 @@
       </c>
       <c r="L11" s="4">
         <v>0.29601948220000002</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="N11" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">

</xml_diff>